<commit_message>
Validation for Create Hockys
</commit_message>
<xml_diff>
--- a/Content/ExcelFiles/Kết quả.xlsx
+++ b/Content/ExcelFiles/Kết quả.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KyThuat88\Documents\TranVietHoang_1621050401\NCKHExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAFC9998-9FF7-4FF7-AA3C-0DBF47609561}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20663AEA-E5BA-4E01-8D65-D081607A5E05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{982FC473-FA66-401E-B0C7-4BF774482B5A}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Update Phân Công Hội Đồng đánh giá kết quả
</commit_message>
<xml_diff>
--- a/Content/ExcelFiles/Kết quả.xlsx
+++ b/Content/ExcelFiles/Kết quả.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KyThuat88\Documents\TranVietHoang_1621050401\NCKHExcelFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20663AEA-E5BA-4E01-8D65-D081607A5E05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD570E57-E172-47EE-AAA0-94DE1F404E69}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{982FC473-FA66-401E-B0C7-4BF774482B5A}"/>
   </bookViews>
@@ -557,7 +557,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>